<commit_message>
opravy v katalogu, moznosti rychleho vykreslovani, moznosti kopirovani
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -1269,7 +1269,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>xlsm</t>
+          <t>xlsx</t>
         </is>
       </c>
     </row>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>80</t>
         </is>
       </c>
     </row>
@@ -1639,6 +1639,13 @@
       <c r="B31" t="inlineStr">
         <is>
           <t>ne</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>precise</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
verze 4.0.1 opravy v prohlížeči obrázků
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -1187,7 +1187,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>C:/Users/jakub.hlavacek.local/Pictures/Screenshots/</t>
+          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Omron/SnímkySC01_MS500SA/</t>
         </is>
       </c>
     </row>
@@ -1503,7 +1503,7 @@
     <row r="20">
       <c r="B20" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>40</t>
         </is>
       </c>
     </row>
@@ -1623,7 +1623,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>100</t>
         </is>
       </c>
     </row>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ano</t>
+          <t>ne</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
více oprav v katalogu
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -1160,7 +1160,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
@@ -1187,7 +1187,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1609,7 +1609,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>xlsx</t>
+          <t>xlsm</t>
         </is>
       </c>
     </row>
@@ -1633,7 +1633,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>60</t>
         </is>
       </c>
     </row>
@@ -1645,7 +1645,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ano</t>
+          <t>ne</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
experimentovani s wraping textboxu, oprava vysky radku - xlsx
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -1160,7 +1160,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -1187,7 +1187,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
vyreseno xlsm a adaptace vysky radku
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -919,7 +919,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
@@ -1123,6 +1123,33 @@
       <c r="D7" t="inlineStr">
         <is>
           <t>ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>529_witte</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>\\192.168.0.192\Data</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Vision</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>*Jhv2708</t>
         </is>
       </c>
     </row>
@@ -1160,7 +1187,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
@@ -1187,7 +1214,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1645,7 +1672,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ne</t>
+          <t>ano</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
dodelani separatniho gui pro disky
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -934,88 +934,94 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>514_Teleflex</t>
+          <t>515_ZF</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>Z</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>\\192.168.14.245\Data\Kamery</t>
+          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Vision</t>
+          <t>jhvadmin</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>*Jhv2708</t>
+          <t>jhvadm1n</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>515_ZF</t>
+          <t>Domaci Nas</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Z</t>
+          <t>S</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>jhvadmin</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>jhvadm1n</t>
+          <t>\\192.168.1.20\Data</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Domaci Nas</t>
+          <t>518_Valeo II</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>VV2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>\\192.168.1.20\Data</t>
+          <t>\\192.168.1.10\10_vision</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Druha sít, ixon
+fj</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>518_Valeo II</t>
+          <t>474_B Austin</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>P</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>\\192.168.1.10\10_vision</t>
+          <t>\\10.96.205.166\DATA</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1025,76 +1031,10 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Jhv*2708</t>
+          <t>*Jhv2708</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
-        <is>
-          <t>Druha sít, ixon
-fj</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>518_Valeo</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>\\192.168.208.200\10_vision</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>první sít, ixon
-\\192.168.208.200\10_vision</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>474_B Austin</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>\\10.96.205.166\DATA</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>*Jhv2708</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
         <is>
           <t>10.96.205.166	
 VisionNas_474B	
@@ -1104,52 +1044,117 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>529_witt</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Wj</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>\\192.168.0.192\Dat</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Visio</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>*Jhv270</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>514_Teleflex</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>\\192.168.14.245\Data\Kamery</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Vision</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>*Jhv2708</t>
+        </is>
+      </c>
+    </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>xfdx</t>
+          <t>518_Valeo</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>VV</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>\\192.168.000.000\</t>
+          <t>\\192.168.208.200\10_vision</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ss</t>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>první sít, ixon
+\\192.168.208.200\10_vision</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>529_witte</t>
+          <t>VUT</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>\\192.168.0.192\Data</t>
+          <t>\\gigadisk2.ro.vutbr.cz\GIGADISK2\home\9\4\0\221049</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Vision</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>*Jhv2708</t>
+          <t>xhlava51@vutbr.cz</t>
         </is>
       </c>
     </row>
@@ -1187,7 +1192,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -1288,14 +1293,80 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A3:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>529_witt</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Wj</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>\\192.168.0.192\Dat</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Visio</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>*Jhv270</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>\\192.168.1.10\10_vision</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Druha sít, ixon
+fj</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1346,7 +1417,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height/</t>
+          <t>C:/Users/kubah/Pictures/Screenshots/</t>
         </is>
       </c>
     </row>
@@ -1564,7 +1635,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ne</t>
+          <t>ano</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
dodělání nové truktury ip setting - zbýva optimalizace IP_assignment
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -501,7 +501,7 @@
 -----------------------------------------
 user:JHV_Vision, omron 
 Pass:*Jhv2708
----------------------------------------j
+---------------------------------------
 FortiClient Austin: 
 Pass:
 1Pm#J@PFIkzM&amp;Q@i 
@@ -604,7 +604,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Kamera VS-S160MX :192.168.0.186</t>
+          <t>Kamera VS-S160MX :192.168.0.18</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -625,12 +625,6 @@
       <c r="C8" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>zv
-zcv</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -712,7 +706,7 @@
       <c r="D11" t="inlineStr">
         <is>
           <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.117f</t>
+OP:		10.101.28.117</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -738,9 +732,8 @@
       <c r="D12" t="inlineStr">
         <is>
           <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
-User:jhvadmin Pass:jhvm1n &gt;&gt;&gt; na portu 8080. 
-123TPV456
-gfsdv</t>
+User:jhvadmin Pass
+123TPV456</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -873,7 +866,7 @@
       <c r="D4" t="inlineStr">
         <is>
           <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.117f</t>
+OP:		10.101.28.117</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -899,9 +892,8 @@
       <c r="D5" t="inlineStr">
         <is>
           <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
-User:jhvadmin Pass:jhvm1n &gt;&gt;&gt; na portu 8080. 
-123TPV456
-gfsdv</t>
+User:jhvadmin Pass
+123TPV456</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -919,7 +911,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
@@ -934,227 +926,193 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>515_ZF</t>
+          <t>514_Teleflex</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Z</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
+          <t>\\192.168.14.245\Data\Kamery</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>jhvadmin</t>
+          <t>Vision</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>jhvadm1n</t>
+          <t>*Jhv2708</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Domaci Nas</t>
+          <t>515_ZF</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>Z</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>\\192.168.1.20\Data</t>
+          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>jhvadmin</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>jhvadm1n</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>518_Valeo II</t>
+          <t>Domaci Nas</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>VV2</t>
+          <t>S</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>\\192.168.1.10\10_vision</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Druha sít, ixon
-fj</t>
+          <t>\\192.168.1.20\Data</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>\\192.168.1.10\10_vision</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Druha sít, ixon</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>518_Valeo</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>\\192.168.208.200\10_vision</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>první sít, ixon
+\\192.168.208.200\10_vision</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>474_B Austin</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>\\10.96.205.166\DATA</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>jhv_vision</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>*Jhv2708</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>10.96.205.166	
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>10.96.205.166
 VisionNas_474B	
 						user:JHV_Vision, omron 
-Pass:*Jhv2708h
-fhjgfds</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>529_witt</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Wj</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>\\192.168.0.192\Dat</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Visio</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>*Jhv270</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>l</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>514_Teleflex</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>T</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>\\192.168.14.245\Data\Kamery</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Vision</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>*Jhv2708</t>
+Pass:*Jhv2708</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>518_Valeo</t>
+          <t>xfdx</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>VV</t>
+          <t>P</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>\\192.168.208.200\10_vision</t>
+          <t>\\192.168.000.000\</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>první sít, ixon
-\\192.168.208.200\10_vision</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>VUT</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>\\gigadisk2.ro.vutbr.cz\GIGADISK2\home\9\4\0\221049</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>xhlava51@vutbr.cz</t>
+          <t>ss</t>
         </is>
       </c>
     </row>
@@ -1293,80 +1251,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:F4"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>529_witt</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Wj</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>\\192.168.0.192\Dat</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Visio</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>*Jhv270</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>l</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>518_Valeo II</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>\\192.168.1.10\10_vision</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Druha sít, ixon
-fj</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1417,7 +1309,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>C:/Users/kubah/Pictures/Screenshots/</t>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -1611,7 +1503,7 @@
     <row r="20">
       <c r="B20" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>85</t>
         </is>
       </c>
     </row>
@@ -1707,7 +1599,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>xlsm</t>
+          <t>xlsx</t>
         </is>
       </c>
     </row>
@@ -1726,13 +1618,11 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>nastavení celkového zoomu [%]:</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+          <t>nastavení zoomu celé aplikace (default: 100 %)</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="31">

</xml_diff>

<commit_message>
dodelani prepisovani struktury u ip setting, oprava unfocus
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -654,20 +654,46 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>527_Teijin</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>10.101.28.176</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>XG-X2900:		10.101.28.175
+OP:		10.101.28.117</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>474 B_Austin</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>10.96.205.175</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
@@ -683,34 +709,8 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>527_Teijin</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>10.101.28.176</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.117</t>
-        </is>
-      </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -751,7 +751,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:E5"/>
@@ -814,12 +814,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>474 B_Austin</t>
+          <t>527_Teijin</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10.96.205.175</t>
+          <t>10.101.28.176</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -828,75 +828,12 @@
         </is>
       </c>
       <c r="D3" t="inlineStr">
-        <is>
-          <t>PC:	10.96.205.175
-NAS:	10.96.205.166
-FH:	10.96.205.154
-	10.96.205.245
------------------------------------------
-user:JHV_Vision, omron 
-Pass:*Jhv2708
----------------------------------------
-FortiClient Austin: 
-Pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>527_Teijin</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>10.101.28.176</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
         <is>
           <t>XG-X2900:		10.101.28.175
 OP:		10.101.28.117</t>
         </is>
       </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>515_ZF Stara Boleslav</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>10.9.250.240</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
-User:jhvadmin Pass
-123TPV456</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
+      <c r="E3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1150,7 +1087,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">
@@ -1251,14 +1188,75 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A3:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>515_ZF Stara Boleslav</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>10.9.250.240</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
+User:jhvadmin Pass
+123TPV456</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>518_Valeo</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>\\192.168.208.200\10_vision</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>první sít, ixon
+\\192.168.208.200\10_vision</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
práce na možnosti nastavit automatické spouštění mazání
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -1307,7 +1307,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
         </is>
       </c>
     </row>
@@ -1619,8 +1619,10 @@
           <t>nastavení zoomu celé aplikace (default: 100 %)</t>
         </is>
       </c>
-      <c r="B30" t="n">
-        <v>100</v>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
       </c>
     </row>
     <row r="31">

</xml_diff>

<commit_message>
nova kontext nabidka v ip setting
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -406,7 +406,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:E12"/>
@@ -515,12 +515,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>511_Teleflex</t>
+          <t>514_Teleflex</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>192.168.1.242</t>
+          <t>192.168.14.240</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -529,31 +529,6 @@
         </is>
       </c>
       <c r="D4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Teleflex </t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>514_Teleflex</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>192.168.14.240</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
         <is>
           <t>PC:192.168.14.240
 CAM: 192.168.14.??NAS:192.168.14.245
@@ -562,19 +537,39 @@
 pass: *Jhv2708</t>
         </is>
       </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>518_Valeo</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>192.168.208.242</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>518_Valeo</t>
+          <t>518_Valeo II</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>192.168.208.242</t>
+          <t>192.168.1.243</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -583,18 +578,18 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>529_Witte</t>
+          <t>474 B_Austin</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>192.168.0.240</t>
+          <t>10.96.205.175</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -603,97 +598,6 @@
         </is>
       </c>
       <c r="D7" t="inlineStr">
-        <is>
-          <t>Kamera VS-S160MX :192.168.0.18</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Domaci Wifi</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>192.168.1.131</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>518_Valeo II</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>192.168.1.243</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>527_Teijin</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>10.101.28.176</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.117</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>474 B_Austin</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>10.96.205.175</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
@@ -709,34 +613,150 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
-      <c r="E11" t="n">
+      <c r="E7" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>515_ZF Stara Boleslav</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Domaci Wifi</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>192.168.1.131</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>527_Teijin</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>10.101.28.176</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>XG-X2900:		10.101.28.175
+OP:		10.101.28.117</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>515_ZF Stara kkkBoleslav</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>10.9.250.240</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
 User:jhvadmin Pass
 123TPV456</t>
         </is>
       </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">515_ </t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>529_Witte</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>192.168.0.240</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Kamera VS-S160MX :192.168.0.18</t>
+        </is>
+      </c>
       <c r="E12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>511_Teleflex</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>192.168.1.242</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Teleflex </t>
+        </is>
+      </c>
+      <c r="E13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -751,7 +771,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:E5"/>
@@ -834,6 +854,53 @@
         </is>
       </c>
       <c r="E3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>515_ZF Stara kkkBoleslav</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>10.9.250.240</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
+User:jhvadmin Pass
+123TPV456</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">515_ </t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1087,7 +1154,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -1114,7 +1181,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1188,7 +1255,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:F4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1196,31 +1263,56 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>515_ZF Stara Boleslav</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>10.9.250.240</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
         <is>
           <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
 User:jhvadmin Pass
 123TPV456</t>
         </is>
       </c>
-      <c r="E3" t="n">
-        <v>1</v>
+      <c r="E1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>511_Teleflex</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>192.168.1.242</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Teleflex </t>
+        </is>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
hodne prace na nastaveni moznosti mazani pres task scheduler, kontext nabidka v tray...
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -420,7 +420,7 @@
       <selection activeCell="A12" sqref="A12:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="27.28515625" customWidth="1" min="1" max="1"/>
     <col width="30.7109375" customWidth="1" min="2" max="2"/>
@@ -785,7 +785,7 @@
       <selection activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15.5703125" customWidth="1" min="3" max="3"/>
   </cols>
@@ -929,7 +929,7 @@
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8.42578125" customWidth="1" min="2" max="2"/>
     <col width="32" customWidth="1" min="3" max="3"/>
@@ -1149,7 +1149,7 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="48.5703125" customWidth="1" min="1" max="1"/>
     <col width="71.7109375" customWidth="1" min="2" max="2"/>
@@ -1760,13 +1760,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="19.5703125" customWidth="1" min="1" max="1"/>
     <col width="78.28515625" customWidth="1" min="2" max="2"/>
@@ -1775,7 +1775,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>TRIMAZKON_task_4</t>
+          <t>TRIMAZKON_task_2</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -1785,54 +1785,105 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>278</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>998</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>12:00:00</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>[1500,datum,soubor1,soubor2,soubor3,…]</t>
-        </is>
-      </c>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>TRIMAZKON_task_3</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>TRIMAZKON_task_1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>30</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>500</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>23:59</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
-    </row>
-    <row r="3"/>
+      <c r="F3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>TRIMAZKON_task_4</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>278</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>998</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1:00</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dodelani ukladani tasku, pridani casu pridani tasku, prace na nastaveni startup tasku pred admina
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -36,12 +36,6 @@
       <color theme="10"/>
       <sz val="11"/>
       <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -420,7 +414,7 @@
       <selection activeCell="A12" sqref="A12:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="27.28515625" customWidth="1" min="1" max="1"/>
     <col width="30.7109375" customWidth="1" min="2" max="2"/>
@@ -785,7 +779,7 @@
       <selection activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="15.5703125" customWidth="1" min="3" max="3"/>
   </cols>
@@ -929,7 +923,7 @@
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="8.42578125" customWidth="1" min="2" max="2"/>
     <col width="32" customWidth="1" min="3" max="3"/>
@@ -1149,7 +1143,7 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="48.5703125" customWidth="1" min="1" max="1"/>
     <col width="71.7109375" customWidth="1" min="2" max="2"/>
@@ -1760,13 +1754,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="19.5703125" customWidth="1" min="1" max="1"/>
     <col width="78.28515625" customWidth="1" min="2" max="2"/>
@@ -1775,115 +1769,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>TRIMAZKON_task_2</t>
+          <t>TRIMAZKON_task_1</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
+          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>278</t>
+          <t>111</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>998</t>
+          <t>5055</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr"/>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>TRIMAZKON_task_3</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>TRIMAZKON_task_1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>23:59</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>TRIMAZKON_task_4</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>278</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>998</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1:00</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-    </row>
+          <t>12:59</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>10.12.2024 15:15:56</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr"/>
+    </row>
+    <row r="2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
zamotani se - include exe souboru - muzu i classu
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -414,7 +414,7 @@
       <selection activeCell="A12" sqref="A12:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="27.28515625" customWidth="1" min="1" max="1"/>
     <col width="30.7109375" customWidth="1" min="2" max="2"/>
@@ -779,7 +779,7 @@
       <selection activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15.5703125" customWidth="1" min="3" max="3"/>
   </cols>
@@ -923,7 +923,7 @@
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8.42578125" customWidth="1" min="2" max="2"/>
     <col width="32" customWidth="1" min="3" max="3"/>
@@ -1143,7 +1143,7 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="48.5703125" customWidth="1" min="1" max="1"/>
     <col width="71.7109375" customWidth="1" min="2" max="2"/>
@@ -1193,7 +1193,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1754,52 +1754,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="E1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="19.5703125" customWidth="1" min="1" max="1"/>
     <col width="78.28515625" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>TRIMAZKON_task_1</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>5055</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>12:59</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>10.12.2024 15:15:56</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr"/>
-    </row>
-    <row r="2"/>
+      <c r="E1" s="2" t="n"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dodelani vizualizace zobrazeni logu + oprava logiky zapisovani
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28695" yWindow="2040" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ip_address_list" sheetId="1" state="visible" r:id="rId1"/>
@@ -22,7 +22,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -37,6 +37,13 @@
       <sz val="11"/>
       <u val="single"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <charset val="238"/>
+      <family val="3"/>
+      <color rgb="FFCE9178"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -60,10 +67,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1754,10 +1764,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="E1:E1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1767,9 +1777,118 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="E1" s="2" t="n"/>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>TRIMAZKON_task_3</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>292</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>17.12.2024 16:11:56</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>|||Datum provedení: 17.12.2024 16:12:19||Zkontrolováno: 161 souborů||Starších:      153 souborů||Smazáno:       103 souborů</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TRIMAZKON_task_2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>292</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>998</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>17.12.2024 10:12:10</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>|||Datum: 17.122222210:12:26||Zkontrolováno: 161 souborů||Starších: 153 souborů||Smazáno: 0 souborů|||Datum: 17.12.2024 10:12:26||Zkontrolováno: 161 souborů||Starších: 153 souborů||Smazáno: 0 souborů</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TRIMAZKON_task_1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>17.12.2024 16:03:53</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>|||Datum provedení: 17.12.2024 16:04:58||Zkontrolováno: 161 souborů||Starších:      153 souborů||Smazáno:       0 souborů|||Datum provedení: 17.12.2024 16:05:16||Zkontrolováno: 161 souborů||Starších:      153 souborů||Smazáno:       0 souborů|||Datum provedení: 17.12.2024 16:08:31||Zkontrolováno: 161 souborů||Starších:      153 souborů||Smazáno:       0 souborů|||Datum provedení: 17.12.2024 16:17:29||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
testování + nové možnosti tray, nový pyinstaller command
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="9600" yWindow="1605" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ip_address_list" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Settings" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="projects_bin2" sheetId="5" state="hidden" r:id="rId5"/>
     <sheet name="Settings_recources" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="task_settings" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Task_settings" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1767,7 +1767,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="G1" s="3" t="inlineStr">
         <is>
-          <t>|||Datum provedení: 17.12.2024 16:12:19||Zkontrolováno: 161 souborů||Starších:      153 souborů||Smazáno:       103 souborů</t>
+          <t>|||Datum provedení: 17.12.2024 16:12:19||Zkontrolováno: 161 souborů||Starších:      153 souborů||Smazáno:       103 souborů|||Datum provedení: 18.12.2024 14:14:10||Zkontrolováno: 108 souborů||Starších: 100 souborů||Smazáno: 50 souborů</t>
         </is>
       </c>
     </row>
@@ -1844,11 +1844,7 @@
           <t>17.12.2024 10:12:10</t>
         </is>
       </c>
-      <c r="G2" s="3" t="inlineStr">
-        <is>
-          <t>|||Datum: 17.122222210:12:26||Zkontrolováno: 161 souborů||Starších: 153 souborů||Smazáno: 0 souborů|||Datum: 17.12.2024 10:12:26||Zkontrolováno: 161 souborů||Starších: 153 souborů||Smazáno: 0 souborů</t>
-        </is>
-      </c>
+      <c r="G2" s="3" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1883,7 +1879,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>|||Datum provedení: 17.12.2024 16:04:58||Zkontrolováno: 161 souborů||Starších:      153 souborů||Smazáno:       0 souborů|||Datum provedení: 17.12.2024 16:05:16||Zkontrolováno: 161 souborů||Starších:      153 souborů||Smazáno:       0 souborů|||Datum provedení: 17.12.2024 16:08:31||Zkontrolováno: 161 souborů||Starších:      153 souborů||Smazáno:       0 souborů|||Datum provedení: 17.12.2024 16:17:29||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů</t>
+          <t>|||Datum provedení: 18.12.2024 14:13:13||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 18.12.2024 14:33:24||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
predelani tray na zvlast exe aplikaci, hláška o configu, prohlizec obrazku predelan na pack a pridana historie cest, prace na otevreni obrazku v novem okne
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -1166,7 +1166,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
@@ -1193,7 +1193,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -1203,7 +1203,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -1605,7 +1605,7 @@
     <row r="20">
       <c r="B20" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>40</t>
         </is>
       </c>
     </row>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="G1" s="3" t="inlineStr">
         <is>
-          <t>|||Datum provedení: 17.12.2024 16:12:19||Zkontrolováno: 161 souborů||Starších:      153 souborů||Smazáno:       103 souborů|||Datum provedení: 18.12.2024 14:14:10||Zkontrolováno: 108 souborů||Starších: 100 souborů||Smazáno: 50 souborů</t>
+          <t>|||Datum provedení: 17.12.2024 16:12:19||Zkontrolováno: 161 souborů||Starších:      153 souborů||Smazáno:       103 souborů|||Datum provedení: 18.12.2024 14:14:10||Zkontrolováno: 108 souborů||Starších: 100 souborů||Smazáno: 50 souborů|||Datum provedení: 20.12.2024 12:00:23||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 08:49:27||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 08:49:43||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 12:00:19||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 14:21:35||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů</t>
         </is>
       </c>
     </row>
@@ -1844,7 +1844,11 @@
           <t>17.12.2024 10:12:10</t>
         </is>
       </c>
-      <c r="G2" s="3" t="inlineStr"/>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>|||Datum provedení: 20.12.2024 12:00:14||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 12:00:10||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1879,7 +1883,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>|||Datum provedení: 18.12.2024 14:13:13||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 18.12.2024 14:33:24||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů</t>
+          <t>|||Datum provedení: 18.12.2024 14:13:13||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 18.12.2024 14:33:24||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 08:55:50||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 08:56:02||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 09:18:00||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 09:36:54||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 10:06:31||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 10:34:32||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 11:02:39||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
práce na tray otevirani v nastaveni aplikace, dodelani otevirani obrazku v novem okne, optimalizace nacitani widgetu u disků
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:E12"/>
@@ -769,6 +769,26 @@
         </is>
       </c>
       <c r="E13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>533valeo</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>192.168.227.27</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E14" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1166,7 +1186,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">
@@ -1193,7 +1213,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1305,22 +1325,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>511_Teleflex</t>
+          <t>533valeo</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>192.168.1.242</t>
+          <t>192.168.277.27</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Teleflex </t>
         </is>
       </c>
       <c r="E3" t="b">
@@ -1371,7 +1386,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1750,6 +1765,18 @@
       <c r="B32" t="inlineStr">
         <is>
           <t>fast</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Nastavení spouštění TRIMAZKON v nabídce system tray</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ano</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
release verze 4.2.0 a znevidetelnene heslo u disků
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -947,7 +947,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
@@ -1151,6 +1151,34 @@
           <t>ss</t>
         </is>
       </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>testetsta</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>\\192.168.000.000\</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>adf</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1213,7 +1241,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -1791,7 +1819,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
@@ -1806,7 +1834,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>TRIMAZKON_task_3</t>
+          <t>TRIMAZKON_task_6</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -1816,12 +1844,12 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>292</t>
+          <t>320</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>998</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
@@ -1831,19 +1859,15 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>17.12.2024 16:11:56</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>|||Datum provedení: 17.12.2024 16:12:19||Zkontrolováno: 161 souborů||Starších:      153 souborů||Smazáno:       103 souborů|||Datum provedení: 18.12.2024 14:14:10||Zkontrolováno: 108 souborů||Starších: 100 souborů||Smazáno: 50 souborů|||Datum provedení: 20.12.2024 12:00:23||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 08:49:27||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 08:49:43||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 12:00:19||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 14:21:35||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů</t>
-        </is>
-      </c>
+          <t>14.01.2025 09:48:31</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TRIMAZKON_task_2</t>
+          <t>TRIMAZKON_task_4</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1853,7 +1877,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>292</t>
+          <t>320</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1868,14 +1892,10 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>17.12.2024 10:12:10</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="inlineStr">
-        <is>
-          <t>|||Datum provedení: 20.12.2024 12:00:14||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 12:00:10||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů</t>
-        </is>
-      </c>
+          <t>14.01.2025 09:44:04</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1911,6 +1931,112 @@
       <c r="G3" t="inlineStr">
         <is>
           <t>|||Datum provedení: 18.12.2024 14:13:13||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 18.12.2024 14:33:24||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 08:55:50||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 08:56:02||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 09:18:00||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 09:36:54||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 10:06:31||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 10:34:32||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 11:02:39||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>TRIMAZKON_task_2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>292</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>998</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>17.12.2024 10:12:10</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>|||Datum provedení: 20.12.2024 12:00:14||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 12:00:10||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TRIMAZKON_task_3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>292</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>17.12.2024 16:11:56</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>|||Datum provedení: 17.12.2024 16:12:19||Zkontrolováno: 161 souborů||Starších:      153 souborů||Smazáno:       103 souborů|||Datum provedení: 18.12.2024 14:14:10||Zkontrolováno: 108 souborů||Starších: 100 souborů||Smazáno: 50 souborů|||Datum provedení: 20.12.2024 12:00:23||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 08:49:27||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 08:49:43||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 12:00:19||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 14:21:35||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TRIMAZKON_task_5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>320</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>5:55</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>14.01.2025 09:44:29</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
velké úpravy v ip settings, oprava deleting, práce na pipeline serveru
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -424,7 +424,7 @@
       <selection activeCell="A12" sqref="A12:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="27.28515625" customWidth="1" min="1" max="1"/>
     <col width="30.7109375" customWidth="1" min="2" max="2"/>
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>440_Austin</t>
+          <t>518_Valeo</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>10.96.205.240</t>
+          <t>192.168.208.242</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -449,29 +449,19 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>FortiClient Austin: 
-pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK
-FH-2050-20
-10.96.205.80</t>
-        </is>
-      </c>
       <c r="E1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>497_Edcha</t>
+          <t>503_Witte</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>172.26.7.240</t>
+          <t>192.168.0.240</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -480,31 +470,6 @@
         </is>
       </c>
       <c r="D2" t="inlineStr">
-        <is>
-          <t>FortiClient Edcha Ex2p78kxp30</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>503_Witte</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>192.168.0.240</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
@@ -520,27 +485,27 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="E2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>514_Teleflex</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>192.168.14.240</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>PC:192.168.14.240
 CAM: 192.168.14.??NAS:192.168.14.245
@@ -549,6 +514,32 @@
 pass: *Jhv2708</t>
         </is>
       </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>527_Teijin</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>10.101.28.176</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>XG-X2900:		10.101.28.175
+OP:		10.101.28.117</t>
+        </is>
+      </c>
       <c r="E4" t="n">
         <v>1</v>
       </c>
@@ -556,12 +547,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>518_Valeo</t>
+          <t>518_Valeo II</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>192.168.208.242</t>
+          <t>192.168.1.243</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -570,18 +561,18 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>518_Valeo II</t>
+          <t>474 B_Austin</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>192.168.1.243</t>
+          <t>10.96.205.175</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -589,27 +580,7 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>474 B_Austin</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>10.96.205.175</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
@@ -625,19 +596,44 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>529_Witte</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>192.168.0.240</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Kamera VS-S160MX :192.168.0.18</t>
+        </is>
+      </c>
+      <c r="E7" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Domaci Wifi</t>
+          <t>511_Teleflex</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>192.168.1.131</t>
+          <t>192.168.1.242</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -645,19 +641,24 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E8" t="n">
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Teleflex d</t>
+        </is>
+      </c>
+      <c r="E8" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>527_Teijin</t>
+          <t>515_ZF Stara kkkBoleslav</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10.101.28.176</t>
+          <t>10.9.250.240</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -666,40 +667,34 @@
         </is>
       </c>
       <c r="D9" t="inlineStr">
-        <is>
-          <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.117</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>515_ZF Stara kkkBoleslav</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>10.9.250.240</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
         <is>
           <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
 User:jhvadmin Pass
 123TPV456</t>
         </is>
       </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Domaci Wifi</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>192.168.1.131</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -719,18 +714,18 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>529_Witte</t>
+          <t>440_Austin</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>192.168.0.240</t>
+          <t>10.96.205.240</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -740,7 +735,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Kamera VS-S160MX :192.168.0.18</t>
+          <t>FortiClient Austin: 
+pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK
+FH-2050-20
+10.96.205.80</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -750,12 +750,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>511_Teleflex</t>
+          <t>497_Edcha</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>192.168.1.242</t>
+          <t>172.26.7.240</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -765,10 +765,10 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Teleflex </t>
-        </is>
-      </c>
-      <c r="E13" t="b">
+          <t>FortiClient Edcha Ex2p78kxp30</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -788,7 +788,7 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E14" t="b">
+      <c r="E14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -809,7 +809,7 @@
       <selection activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="15.5703125" customWidth="1" min="3" max="3"/>
   </cols>
@@ -817,12 +817,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>518_Valeo II</t>
+          <t>514_Teleflex</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.1.243</t>
+          <t>192.168.14.240</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -830,33 +830,33 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>514_Teleflex</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>192.168.14.240</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>PC:192.168.14.240
 CAM: 192.168.14.??NAS:192.168.14.245
 *******************************
 user: Vision
 pass: *Jhv2708</t>
+        </is>
+      </c>
+      <c r="E1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>192.168.1.243</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -947,13 +947,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="8.42578125" customWidth="1" min="2" max="2"/>
     <col width="32" customWidth="1" min="3" max="3"/>
@@ -962,166 +962,80 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>514_Teleflex</t>
+          <t>Domaci Nas</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>S</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>\\192.168.14.245\Data\Kamery</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Vision</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>*Jhv2708</t>
+          <t>\\192.168.1.20\Data</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>515_ZF</t>
+          <t>518_Valeo</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Z</t>
+          <t>V</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
+          <t>\\192.168.208.200\10_vision</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>jhvadmin</t>
+          <t>jhv_vision</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>jhvadm1n</t>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>první sít, ixon
+\\192.168.208.200\10_vision</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Domaci Nas</t>
+          <t>474_B Austin</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>P</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>\\192.168.1.20\Data</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>518_Valeo II</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>\\192.168.1.10\10_vision</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
+          <t>\\10.96.205.166\DATA</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>jhv_vision</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Druha sít, ixon</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>518_Valeo</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>\\192.168.208.200\10_vision</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>první sít, ixon
-\\192.168.208.200\10_vision</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>474_B Austin</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>\\10.96.205.166\DATA</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>*Jhv2708</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>10.96.205.166
 VisionNas_474B	
@@ -1130,55 +1044,108 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>514_Teleflex</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>\\192.168.14.245\Data\Kamery</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Vision</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>*Jhv2708</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>\\192.168.1.10\10_vision</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Druha sít, ixon</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>515_ZF</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>jhvadmin</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>jhvadm1n</t>
+        </is>
+      </c>
+    </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>xfdx</t>
+          <t>witte</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>W</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>\\192.168.000.000\</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>ss</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>testetsta</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>\\192.168.000.000\</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>aa</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>adf</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>\\192.168.0.192\</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1201,7 +1168,7 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="48.5703125" customWidth="1" min="1" max="1"/>
     <col width="71.7109375" customWidth="1" min="2" max="2"/>
@@ -1214,7 +1181,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
@@ -1291,7 +1258,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1350,15 +1317,42 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>514_Teleflexx</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>\\192.168.14.245\Data\Kamery</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Vision</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>*Jhv2708</t>
+        </is>
+      </c>
+    </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>533valeo</t>
+          <t>515_ZF Stara kkkBoleslav</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>192.168.277.27</t>
+          <t>10.9.250.240</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1366,8 +1360,15 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E3" t="b">
-        <v>0</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
+User:jhvadmin Pass
+123TPV456</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1819,227 +1820,30 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="19.5703125" customWidth="1" min="1" max="1"/>
     <col width="78.28515625" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>TRIMAZKON_task_6</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>320</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>998</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>14.01.2025 09:48:31</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="G1" s="3" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>TRIMAZKON_task_4</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>320</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>998</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>14.01.2025 09:44:04</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>TRIMAZKON_task_1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>6:00</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>17.12.2024 16:03:53</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>|||Datum provedení: 18.12.2024 14:13:13||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 18.12.2024 14:33:24||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 08:55:50||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 08:56:02||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 09:18:00||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 09:36:54||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 10:06:31||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 10:34:32||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 11:02:39||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>TRIMAZKON_task_2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>292</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>998</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>17.12.2024 10:12:10</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>|||Datum provedení: 20.12.2024 12:00:14||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 12:00:10||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>TRIMAZKON_task_3</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>292</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>17.12.2024 16:11:56</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>|||Datum provedení: 17.12.2024 16:12:19||Zkontrolováno: 161 souborů||Starších:      153 souborů||Smazáno:       103 souborů|||Datum provedení: 18.12.2024 14:14:10||Zkontrolováno: 108 souborů||Starších: 100 souborů||Smazáno: 50 souborů|||Datum provedení: 20.12.2024 12:00:23||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 08:49:27||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 08:49:43||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 12:00:19||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů|||Datum provedení: 03.01.2025 14:21:35||Zkontrolováno: 58 souborů||Starších: 50 souborů||Smazáno: 0 souborů</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>TRIMAZKON_task_5</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>320</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>5:55</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>14.01.2025 09:44:29</t>
-        </is>
-      </c>
-    </row>
+      <c r="G2" s="3" t="n"/>
+    </row>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
release verze 4.2.1 a práce na samostatném mazání - vývoj komunikace pipeline
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -424,7 +424,7 @@
       <selection activeCell="A12" sqref="A12:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="27.28515625" customWidth="1" min="1" max="1"/>
     <col width="30.7109375" customWidth="1" min="2" max="2"/>
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>518_Valeo</t>
+          <t>Domaci Wifi</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.208.242</t>
+          <t>192.168.1.131</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -456,20 +456,232 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>533valeo</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>192.168.227.27</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>529_Witte</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>192.168.0.240</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Kamera VS-S160MX :192.168.0.18</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>527_Teijin</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>10.101.28.176</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>XG-X2900:		10.101.28.175
+OP:		10.101.28.117</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>192.168.1.243</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>518_Valeo</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>192.168.208.242</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>515_ZF Stara kkkBoleslav</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>10.9.250.240</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
+User:jhvadmin Pass
+123TPV456</t>
+        </is>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">515_ </t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>514_Teleflex</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>192.168.14.240</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>PC:192.168.14.240
+CAM: 192.168.14.??NAS:192.168.14.245
+*******************************
+user: Vision
+pass: *Jhv2708</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>511_Teleflex</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>192.168.1.242</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Teleflex d</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>503_Witte</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>192.168.0.240</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
@@ -485,102 +697,52 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="E11" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>514_Teleflex</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>192.168.14.240</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>PC:192.168.14.240
-CAM: 192.168.14.??NAS:192.168.14.245
-*******************************
-user: Vision
-pass: *Jhv2708</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>527_Teijin</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>10.101.28.176</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.117</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>518_Valeo II</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>192.168.1.243</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>497_Edcha</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>172.26.7.240</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>FortiClient Edcha Ex2p78kxp30</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
         <is>
           <t>474 B_Austin</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>10.96.205.175</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
@@ -596,144 +758,27 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="E13" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>529_Witte</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>192.168.0.240</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Kamera VS-S160MX :192.168.0.18</t>
-        </is>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>511_Teleflex</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>192.168.1.242</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Teleflex d</t>
-        </is>
-      </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>515_ZF Stara kkkBoleslav</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>10.9.250.240</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
-User:jhvadmin Pass
-123TPV456</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Domaci Wifi</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>192.168.1.131</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">515_ </t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>192.168.000.000</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+    <row r="14">
+      <c r="A14" t="inlineStr">
         <is>
           <t>440_Austin</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>10.96.205.240</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>FortiClient Austin: 
 pass:
@@ -741,51 +786,6 @@
 UVt1@Ex2p78kxp30atD7we@!qGK
 FH-2050-20
 10.96.205.80</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>497_Edcha</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>172.26.7.240</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>FortiClient Edcha Ex2p78kxp30</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>533valeo</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>192.168.227.27</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -809,7 +809,7 @@
       <selection activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15.5703125" customWidth="1" min="3" max="3"/>
   </cols>
@@ -817,119 +817,119 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>527_Teijin</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>10.101.28.176</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>XG-X2900:		10.101.28.175
+OP:		10.101.28.117</t>
+        </is>
+      </c>
+      <c r="E1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>192.168.1.243</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>515_ZF Stara kkkBoleslav</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>10.9.250.240</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
+User:jhvadmin Pass
+123TPV456</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">515_ </t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>514_Teleflex</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>192.168.14.240</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>PC:192.168.14.240
 CAM: 192.168.14.??NAS:192.168.14.245
 *******************************
 user: Vision
 pass: *Jhv2708</t>
-        </is>
-      </c>
-      <c r="E1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>518_Valeo II</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>192.168.1.243</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>527_Teijin</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>10.101.28.176</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.117</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>515_ZF Stara kkkBoleslav</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>10.9.250.240</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
-User:jhvadmin Pass
-123TPV456</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">515_ </t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>192.168.000.000</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -953,7 +953,7 @@
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8.42578125" customWidth="1" min="2" max="2"/>
     <col width="32" customWidth="1" min="3" max="3"/>
@@ -962,188 +962,191 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Domaci Nas</t>
+          <t>witte</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>W</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>\\192.168.1.20\Data</t>
-        </is>
-      </c>
+          <t>\\192.168.0.192\</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr"/>
+      <c r="E1" t="inlineStr"/>
+      <c r="F1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Domaci Nas</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>\\192.168.1.20\Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>\\192.168.1.10\10_vision</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Druha sít, ixon</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>518_Valeo</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>V</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>\\192.168.208.200\10_vision</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>jhv_vision</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Jhv*2708</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>první sít, ixon
 \\192.168.208.200\10_vision</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>515_ZF</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>jhvadmin</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>jhvadm1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>514_Teleflex</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>\\192.168.14.245\Data\Kamery</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Vision</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>*Jhv2708</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>474_B Austin</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>\\10.96.205.166\DATA</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>jhv_vision</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>*Jhv2708</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>10.96.205.166
 VisionNas_474B	
 						user:JHV_Vision, omron 
 Pass:*Jhv2708</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>514_Teleflex</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>T</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>\\192.168.14.245\Data\Kamery</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Vision</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>*Jhv2708</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>518_Valeo II</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>\\192.168.1.10\10_vision</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Druha sít, ixon</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>515_ZF</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>jhvadmin</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>jhvadm1n</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>witte</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>\\192.168.0.192\</t>
         </is>
       </c>
     </row>
@@ -1168,7 +1171,7 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="48.5703125" customWidth="1" min="1" max="1"/>
     <col width="71.7109375" customWidth="1" min="2" max="2"/>
@@ -1198,7 +1201,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1820,13 +1823,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="E1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="19.5703125" customWidth="1" min="1" max="1"/>
     <col width="78.28515625" customWidth="1" min="2" max="2"/>
@@ -1839,11 +1842,6 @@
     <row r="2">
       <c r="G2" s="3" t="n"/>
     </row>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
prace na novem configu - prevzata kompletni logika z tray z jhv_MAZ
</commit_message>
<xml_diff>
--- a/TRIMAZKON/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/config_TRIMAZKON.xlsx
@@ -975,9 +975,6 @@
           <t>\\192.168.0.192\</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr"/>
-      <c r="E1" t="inlineStr"/>
-      <c r="F1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1211,7 +1208,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1808,7 +1805,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ano</t>
+          <t>ne</t>
         </is>
       </c>
     </row>

</xml_diff>